<commit_message>
added gps and fall tracking
</commit_message>
<xml_diff>
--- a/Data-Sheets-Excels/Mappe1.xlsx
+++ b/Data-Sheets-Excels/Mappe1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hardware\Project-Airframe\Data-Sheets-Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC3B3B6-95E9-4BD7-AB1D-30DBF7F8CC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A20225A-F772-46F7-98D2-AAE8774CF577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22965" yWindow="915" windowWidth="21690" windowHeight="15135" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
+    <workbookView xWindow="22965" yWindow="915" windowWidth="26280" windowHeight="15135" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,8 +65,15 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -76,6 +83,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -92,12 +105,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -333,7 +348,7 @@
                   <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>102</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>80</c:v>
@@ -2521,10 +2536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B586C1-A708-43CB-9379-D0B63D1A81A1}">
-  <dimension ref="A1:H267"/>
+  <dimension ref="A1:H276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F250" sqref="F250"/>
+    <sheetView tabSelected="1" topLeftCell="A262" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F273" sqref="F273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2824,7 +2839,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44823</v>
       </c>
@@ -2834,7 +2849,7 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44824</v>
       </c>
@@ -2844,7 +2859,7 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>44825</v>
       </c>
@@ -2854,7 +2869,7 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44826</v>
       </c>
@@ -2864,7 +2879,7 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44827</v>
       </c>
@@ -2874,7 +2889,7 @@
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>44828</v>
       </c>
@@ -2884,7 +2899,7 @@
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>44829</v>
       </c>
@@ -2896,8 +2911,9 @@
         <f>SUM(B33:B39) + 42</f>
         <v>47</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="5"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>44830</v>
       </c>
@@ -2907,7 +2923,7 @@
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>44831</v>
       </c>
@@ -2917,7 +2933,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>44832</v>
       </c>
@@ -2927,7 +2943,7 @@
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>44833</v>
       </c>
@@ -2937,7 +2953,7 @@
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44834</v>
       </c>
@@ -2947,7 +2963,7 @@
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>44835</v>
       </c>
@@ -2957,7 +2973,7 @@
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44836</v>
       </c>
@@ -2969,6 +2985,7 @@
         <f>SUM(B41:B47) + 42</f>
         <v>52</v>
       </c>
+      <c r="E47" s="5"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
@@ -3262,7 +3279,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>44865</v>
       </c>
@@ -3272,7 +3289,7 @@
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>44866</v>
       </c>
@@ -3282,7 +3299,7 @@
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>44867</v>
       </c>
@@ -3292,7 +3309,7 @@
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>44868</v>
       </c>
@@ -3302,7 +3319,7 @@
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>44869</v>
       </c>
@@ -3312,7 +3329,7 @@
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>44870</v>
       </c>
@@ -3322,7 +3339,7 @@
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>44871</v>
       </c>
@@ -3335,7 +3352,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>44871</v>
       </c>
@@ -3345,7 +3362,7 @@
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>44872</v>
       </c>
@@ -3355,7 +3372,7 @@
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>44873</v>
       </c>
@@ -3365,7 +3382,7 @@
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>44874</v>
       </c>
@@ -3375,7 +3392,7 @@
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>44875</v>
       </c>
@@ -3385,7 +3402,7 @@
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>44876</v>
       </c>
@@ -3395,7 +3412,7 @@
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>44877</v>
       </c>
@@ -3405,7 +3422,7 @@
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>44878</v>
       </c>
@@ -3415,6 +3432,7 @@
         <f>SUM(B90:B96) + 42</f>
         <v>48</v>
       </c>
+      <c r="E96" s="5"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
@@ -3859,8 +3877,8 @@
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3">
-        <f>SUM(B138:B144) + 42</f>
-        <v>102</v>
+        <f>SUM(B138:B144)</f>
+        <v>60</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -4153,7 +4171,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>44963</v>
       </c>
@@ -4163,7 +4181,7 @@
       <c r="C178" s="2"/>
       <c r="D178" s="2"/>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>44964</v>
       </c>
@@ -4173,7 +4191,7 @@
       <c r="C179" s="2"/>
       <c r="D179" s="2"/>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>44965</v>
       </c>
@@ -4183,7 +4201,7 @@
       <c r="C180" s="2"/>
       <c r="D180" s="2"/>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>44966</v>
       </c>
@@ -4193,7 +4211,7 @@
       <c r="C181" s="2"/>
       <c r="D181" s="2"/>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>44967</v>
       </c>
@@ -4203,7 +4221,7 @@
       <c r="C182" s="2"/>
       <c r="D182" s="2"/>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>44968</v>
       </c>
@@ -4213,7 +4231,7 @@
       <c r="C183" s="2"/>
       <c r="D183" s="2"/>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>44969</v>
       </c>
@@ -4225,8 +4243,9 @@
         <f>SUM(B178:B184) + 42</f>
         <v>58</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E184" s="5"/>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>44970</v>
       </c>
@@ -4236,7 +4255,7 @@
       <c r="C186" s="2"/>
       <c r="D186" s="2"/>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>44971</v>
       </c>
@@ -4246,7 +4265,7 @@
       <c r="C187" s="2"/>
       <c r="D187" s="2"/>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>44972</v>
       </c>
@@ -4256,7 +4275,7 @@
       <c r="C188" s="2"/>
       <c r="D188" s="2"/>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>44973</v>
       </c>
@@ -4266,7 +4285,7 @@
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>44974</v>
       </c>
@@ -4276,7 +4295,7 @@
       <c r="C190" s="2"/>
       <c r="D190" s="2"/>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>44975</v>
       </c>
@@ -4286,7 +4305,7 @@
       <c r="C191" s="2"/>
       <c r="D191" s="2"/>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>44976</v>
       </c>
@@ -4445,7 +4464,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>44991</v>
       </c>
@@ -4455,7 +4474,7 @@
       <c r="C210" s="3"/>
       <c r="D210" s="3"/>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>44992</v>
       </c>
@@ -4465,7 +4484,7 @@
       <c r="C211" s="3"/>
       <c r="D211" s="3"/>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>44993</v>
       </c>
@@ -4475,7 +4494,7 @@
       <c r="C212" s="3"/>
       <c r="D212" s="3"/>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>44994</v>
       </c>
@@ -4485,7 +4504,7 @@
       <c r="C213" s="3"/>
       <c r="D213" s="3"/>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>44995</v>
       </c>
@@ -4495,7 +4514,7 @@
       <c r="C214" s="3"/>
       <c r="D214" s="3"/>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>44996</v>
       </c>
@@ -4505,7 +4524,7 @@
       <c r="C215" s="3"/>
       <c r="D215" s="3"/>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>44997</v>
       </c>
@@ -4518,7 +4537,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>44998</v>
       </c>
@@ -4528,7 +4547,7 @@
       <c r="C218" s="3"/>
       <c r="D218" s="3"/>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>44999</v>
       </c>
@@ -4538,7 +4557,7 @@
       <c r="C219" s="3"/>
       <c r="D219" s="3"/>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>45000</v>
       </c>
@@ -4548,7 +4567,7 @@
       <c r="C220" s="3"/>
       <c r="D220" s="3"/>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>45001</v>
       </c>
@@ -4558,7 +4577,7 @@
       <c r="C221" s="3"/>
       <c r="D221" s="3"/>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>45002</v>
       </c>
@@ -4568,7 +4587,7 @@
       <c r="C222" s="3"/>
       <c r="D222" s="3"/>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>45003</v>
       </c>
@@ -4578,7 +4597,7 @@
       <c r="C223" s="3"/>
       <c r="D223" s="3"/>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>45004</v>
       </c>
@@ -4590,8 +4609,9 @@
         <f>SUM(B218:B224) + 42</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E224" s="5"/>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>45005</v>
       </c>
@@ -4601,7 +4621,7 @@
       <c r="C226" s="3"/>
       <c r="D226" s="3"/>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <v>45006</v>
       </c>
@@ -4611,7 +4631,7 @@
       <c r="C227" s="3"/>
       <c r="D227" s="3"/>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <v>45007</v>
       </c>
@@ -4621,7 +4641,7 @@
       <c r="C228" s="3"/>
       <c r="D228" s="3"/>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>45008</v>
       </c>
@@ -4631,7 +4651,7 @@
       <c r="C229" s="3"/>
       <c r="D229" s="3"/>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
         <v>45009</v>
       </c>
@@ -4641,7 +4661,7 @@
       <c r="C230" s="3"/>
       <c r="D230" s="3"/>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
         <v>45010</v>
       </c>
@@ -4651,7 +4671,7 @@
       <c r="C231" s="3"/>
       <c r="D231" s="3"/>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
         <v>45011</v>
       </c>
@@ -4664,7 +4684,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
         <v>45012</v>
       </c>
@@ -4674,7 +4694,7 @@
       <c r="C234" s="3"/>
       <c r="D234" s="3"/>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
         <v>45013</v>
       </c>
@@ -4684,7 +4704,7 @@
       <c r="C235" s="3"/>
       <c r="D235" s="3"/>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
         <v>45014</v>
       </c>
@@ -4694,7 +4714,7 @@
       <c r="C236" s="3"/>
       <c r="D236" s="3"/>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
         <v>45015</v>
       </c>
@@ -4704,7 +4724,7 @@
       <c r="C237" s="3"/>
       <c r="D237" s="3"/>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
         <v>45016</v>
       </c>
@@ -4714,7 +4734,7 @@
       <c r="C238" s="3"/>
       <c r="D238" s="3"/>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
         <v>45017</v>
       </c>
@@ -4724,7 +4744,7 @@
       <c r="C239" s="3"/>
       <c r="D239" s="3"/>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
         <v>45018</v>
       </c>
@@ -4733,8 +4753,9 @@
       </c>
       <c r="C240" s="3"/>
       <c r="D240" s="3"/>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E240" s="5"/>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
         <v>45019</v>
       </c>
@@ -4744,7 +4765,7 @@
       <c r="C242" s="3"/>
       <c r="D242" s="3"/>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
         <v>45020</v>
       </c>
@@ -4754,7 +4775,7 @@
       <c r="C243" s="3"/>
       <c r="D243" s="3"/>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
         <v>45021</v>
       </c>
@@ -4764,7 +4785,7 @@
       <c r="C244" s="3"/>
       <c r="D244" s="3"/>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
         <v>45022</v>
       </c>
@@ -4774,7 +4795,7 @@
       <c r="C245" s="3"/>
       <c r="D245" s="3"/>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
         <v>45023</v>
       </c>
@@ -4784,7 +4805,7 @@
       <c r="C246" s="3"/>
       <c r="D246" s="3"/>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
         <v>45024</v>
       </c>
@@ -4794,7 +4815,7 @@
       <c r="C247" s="3"/>
       <c r="D247" s="3"/>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
         <v>45025</v>
       </c>
@@ -4807,33 +4828,37 @@
         <v>65</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
         <v>45026</v>
       </c>
       <c r="B250" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C250" s="3"/>
       <c r="D250" s="3"/>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
         <v>45027</v>
       </c>
-      <c r="B251" s="3"/>
+      <c r="B251" s="3">
+        <v>1</v>
+      </c>
       <c r="C251" s="3"/>
       <c r="D251" s="3"/>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="2">
         <v>45028</v>
       </c>
-      <c r="B252" s="3"/>
+      <c r="B252" s="3">
+        <v>1</v>
+      </c>
       <c r="C252" s="3"/>
       <c r="D252" s="3"/>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
         <v>45029</v>
       </c>
@@ -4841,39 +4866,47 @@
       <c r="C253" s="3"/>
       <c r="D253" s="3"/>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
         <v>45030</v>
       </c>
-      <c r="B254" s="3"/>
+      <c r="B254" s="3">
+        <v>3</v>
+      </c>
       <c r="C254" s="3"/>
       <c r="D254" s="3"/>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
         <v>45031</v>
       </c>
-      <c r="B255" s="3"/>
+      <c r="B255" s="3">
+        <v>7</v>
+      </c>
       <c r="C255" s="3"/>
       <c r="D255" s="3"/>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
         <v>45032</v>
       </c>
       <c r="B256" s="3"/>
       <c r="C256" s="3"/>
-      <c r="D256" s="3"/>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A257" s="2">
+      <c r="D256" s="3">
+        <f>SUM(B250:B257) + 42</f>
+        <v>67</v>
+      </c>
+      <c r="E256" s="5"/>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A258" s="2">
         <v>45033</v>
       </c>
-      <c r="B257" s="3"/>
-      <c r="C257" s="3"/>
-      <c r="D257" s="3"/>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B258" s="3"/>
+      <c r="C258" s="3"/>
+      <c r="D258" s="3"/>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="2">
         <v>45034</v>
       </c>
@@ -4881,7 +4914,7 @@
       <c r="C259" s="3"/>
       <c r="D259" s="3"/>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="2">
         <v>45035</v>
       </c>
@@ -4889,7 +4922,7 @@
       <c r="C260" s="3"/>
       <c r="D260" s="3"/>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="2">
         <v>45036</v>
       </c>
@@ -4897,7 +4930,7 @@
       <c r="C261" s="3"/>
       <c r="D261" s="3"/>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="2">
         <v>45037</v>
       </c>
@@ -4905,7 +4938,7 @@
       <c r="C262" s="3"/>
       <c r="D262" s="3"/>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="2">
         <v>45038</v>
       </c>
@@ -4913,34 +4946,85 @@
       <c r="C263" s="3"/>
       <c r="D263" s="3"/>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="2">
         <v>45039</v>
       </c>
       <c r="B264" s="3"/>
       <c r="C264" s="3"/>
       <c r="D264" s="3"/>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A265" s="2">
+      <c r="E264" s="6"/>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A266" s="2">
         <v>45040</v>
       </c>
-      <c r="B265" s="3"/>
-      <c r="C265" s="3"/>
-      <c r="D265" s="3"/>
-    </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B266" s="3"/>
+      <c r="C266" s="3"/>
+      <c r="D266" s="3"/>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A267" s="2">
+        <v>45041</v>
+      </c>
       <c r="B267" s="3">
-        <f>SUM(B2:B265)</f>
-        <v>1071</v>
-      </c>
-      <c r="C267">
-        <f>B267/28</f>
-        <v>38.25</v>
-      </c>
-      <c r="D267">
-        <f>28*7</f>
-        <v>196</v>
+        <v>8</v>
+      </c>
+      <c r="C267" s="3"/>
+      <c r="D267" s="3"/>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A268" s="2">
+        <v>45042</v>
+      </c>
+      <c r="B268" s="3"/>
+      <c r="C268" s="3"/>
+      <c r="D268" s="3"/>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A269" s="2">
+        <v>45043</v>
+      </c>
+      <c r="B269" s="3"/>
+      <c r="C269" s="3"/>
+      <c r="D269" s="3"/>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A270" s="2">
+        <v>45044</v>
+      </c>
+      <c r="B270" s="3"/>
+      <c r="C270" s="3"/>
+      <c r="D270" s="3"/>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A271" s="2">
+        <v>45045</v>
+      </c>
+      <c r="B271" s="3"/>
+      <c r="C271" s="3"/>
+      <c r="D271" s="3"/>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A272" s="2">
+        <v>45046</v>
+      </c>
+      <c r="B272" s="3"/>
+      <c r="C272" s="3"/>
+      <c r="D272" s="3"/>
+    </row>
+    <row r="276" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B276" s="3">
+        <f>SUM(B2:B272)</f>
+        <v>1093</v>
+      </c>
+      <c r="C276">
+        <f>B276/29</f>
+        <v>37.689655172413794</v>
+      </c>
+      <c r="D276">
+        <f>32*7</f>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 2 display watchfaces, added sleep tracker
</commit_message>
<xml_diff>
--- a/Data-Sheets-Excels/Mappe1.xlsx
+++ b/Data-Sheets-Excels/Mappe1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hardware\Project-Airframe\Data-Sheets-Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCB34C7-2FE6-4780-AD44-6326FAE701D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B90DC0-8F09-44F0-BB2E-A1C1A1754BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22965" yWindow="915" windowWidth="26280" windowHeight="15135" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
+    <workbookView xWindow="6345" yWindow="225" windowWidth="26280" windowHeight="15135" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -2536,10 +2536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B586C1-A708-43CB-9379-D0B63D1A81A1}">
-  <dimension ref="A1:H276"/>
+  <dimension ref="A1:H283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B278" sqref="B278"/>
+    <sheetView tabSelected="1" topLeftCell="A268" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F273" sqref="F273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5017,25 +5017,85 @@
       <c r="A272" s="2">
         <v>45046</v>
       </c>
-      <c r="B272" s="3"/>
+      <c r="B272" s="3">
+        <v>12</v>
+      </c>
       <c r="C272" s="3"/>
       <c r="D272" s="3">
         <f>SUM(B266:B273) + 42</f>
-        <v>76</v>
-      </c>
-    </row>
-    <row r="276" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B276" s="3">
-        <f>SUM(B2:B272)</f>
-        <v>1119</v>
-      </c>
-      <c r="C276">
-        <f>B276/29</f>
-        <v>38.586206896551722</v>
-      </c>
-      <c r="D276">
-        <f>32*7</f>
-        <v>224</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" s="2">
+        <v>45047</v>
+      </c>
+      <c r="B274" s="3">
+        <v>11</v>
+      </c>
+      <c r="C274" s="3"/>
+      <c r="D274" s="3"/>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" s="2">
+        <v>45048</v>
+      </c>
+      <c r="B275" s="3"/>
+      <c r="C275" s="3"/>
+      <c r="D275" s="3"/>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" s="2">
+        <v>45049</v>
+      </c>
+      <c r="B276" s="3"/>
+      <c r="C276" s="3"/>
+      <c r="D276" s="3"/>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" s="2">
+        <v>45050</v>
+      </c>
+      <c r="B277" s="3"/>
+      <c r="C277" s="3"/>
+      <c r="D277" s="3"/>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" s="2">
+        <v>45051</v>
+      </c>
+      <c r="B278" s="3"/>
+      <c r="C278" s="3"/>
+      <c r="D278" s="3"/>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" s="2">
+        <v>45052</v>
+      </c>
+      <c r="B279" s="3"/>
+      <c r="C279" s="3"/>
+      <c r="D279" s="3"/>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" s="2">
+        <v>45053</v>
+      </c>
+      <c r="B280" s="3"/>
+      <c r="C280" s="3"/>
+      <c r="D280" s="3"/>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B283" s="3">
+        <f>SUM(B2:B280)</f>
+        <v>1142</v>
+      </c>
+      <c r="C283">
+        <f>B283/30</f>
+        <v>38.06666666666667</v>
+      </c>
+      <c r="D283">
+        <f>34*7</f>
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ECG, Oxy and HeartRate Stats, Sleep Stats and Watch Infos
</commit_message>
<xml_diff>
--- a/Data-Sheets-Excels/Mappe1.xlsx
+++ b/Data-Sheets-Excels/Mappe1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hardware\Project-Airframe\Data-Sheets-Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE5A032-11BF-411D-A184-F6AA196C1A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544A1338-14A6-4D6D-9D48-E1795D413026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23400" yWindow="570" windowWidth="26280" windowHeight="15135" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
+    <workbookView xWindow="8835" yWindow="825" windowWidth="26280" windowHeight="15135" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -2539,7 +2539,7 @@
   <dimension ref="A1:H283"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A265" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B277" sqref="B277"/>
+      <selection activeCell="H280" sqref="H280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5060,7 +5060,9 @@
       <c r="A277" s="2">
         <v>45050</v>
       </c>
-      <c r="B277" s="3"/>
+      <c r="B277" s="3">
+        <v>1</v>
+      </c>
       <c r="C277" s="3"/>
       <c r="D277" s="3"/>
     </row>
@@ -5068,7 +5070,9 @@
       <c r="A278" s="2">
         <v>45051</v>
       </c>
-      <c r="B278" s="3"/>
+      <c r="B278" s="3">
+        <v>7</v>
+      </c>
       <c r="C278" s="3"/>
       <c r="D278" s="3"/>
     </row>
@@ -5076,7 +5080,9 @@
       <c r="A279" s="2">
         <v>45052</v>
       </c>
-      <c r="B279" s="3"/>
+      <c r="B279" s="3">
+        <v>7</v>
+      </c>
       <c r="C279" s="3"/>
       <c r="D279" s="3"/>
     </row>
@@ -5086,16 +5092,19 @@
       </c>
       <c r="B280" s="3"/>
       <c r="C280" s="3"/>
-      <c r="D280" s="3"/>
+      <c r="D280" s="3">
+        <f>SUM(B274:B281) + 42</f>
+        <v>77</v>
+      </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B283" s="3">
         <f>SUM(B2:B280)</f>
-        <v>1151</v>
+        <v>1166</v>
       </c>
       <c r="C283">
         <f>B283/30</f>
-        <v>38.366666666666667</v>
+        <v>38.866666666666667</v>
       </c>
       <c r="D283">
         <f>34*7</f>

</xml_diff>

<commit_message>
Added some .step files
</commit_message>
<xml_diff>
--- a/Data-Sheets-Excels/Mappe1.xlsx
+++ b/Data-Sheets-Excels/Mappe1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hardware\Project-Airframe\Data-Sheets-Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09234583-1538-4271-896F-F3A83F5F7517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202A5CC1-6B5D-4528-9465-C8819B6311AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38730" yWindow="915" windowWidth="18870" windowHeight="15135" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
+    <workbookView xWindow="22545" yWindow="720" windowWidth="18870" windowHeight="15135" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -2536,10 +2536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B586C1-A708-43CB-9379-D0B63D1A81A1}">
-  <dimension ref="A1:H283"/>
+  <dimension ref="A1:H338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G274" sqref="G274"/>
+    <sheetView tabSelected="1" topLeftCell="A313" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D286" sqref="D286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5099,18 +5099,422 @@
         <v>91</v>
       </c>
     </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282" s="2">
+        <v>45054</v>
+      </c>
+      <c r="B282" s="3">
+        <v>5</v>
+      </c>
+      <c r="C282" s="3"/>
+      <c r="D282" s="3"/>
+    </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" s="2">
+        <v>45055</v>
+      </c>
       <c r="B283" s="3">
-        <f>SUM(B2:B280)</f>
-        <v>1180</v>
-      </c>
-      <c r="C283">
-        <f>B283/30</f>
-        <v>39.333333333333336</v>
-      </c>
-      <c r="D283">
-        <f>34*7</f>
-        <v>238</v>
+        <v>7</v>
+      </c>
+      <c r="C283" s="3"/>
+      <c r="D283" s="3"/>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" s="2">
+        <v>45056</v>
+      </c>
+      <c r="B284" s="3">
+        <v>6</v>
+      </c>
+      <c r="C284" s="3"/>
+      <c r="D284" s="3"/>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A285" s="2">
+        <v>45057</v>
+      </c>
+      <c r="B285" s="3">
+        <v>4</v>
+      </c>
+      <c r="C285" s="3"/>
+      <c r="D285" s="3"/>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A286" s="2">
+        <v>45058</v>
+      </c>
+      <c r="B286" s="3">
+        <v>11</v>
+      </c>
+      <c r="C286" s="3"/>
+      <c r="D286" s="3"/>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287" s="2">
+        <v>45059</v>
+      </c>
+      <c r="B287" s="3">
+        <v>6</v>
+      </c>
+      <c r="C287" s="3"/>
+      <c r="D287" s="3"/>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288" s="2">
+        <v>45060</v>
+      </c>
+      <c r="B288" s="3"/>
+      <c r="C288" s="3"/>
+      <c r="D288" s="3"/>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" s="2">
+        <v>45061</v>
+      </c>
+      <c r="B290" s="3"/>
+      <c r="C290" s="3"/>
+      <c r="D290" s="3"/>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" s="2">
+        <v>45062</v>
+      </c>
+      <c r="B291" s="3"/>
+      <c r="C291" s="3"/>
+      <c r="D291" s="3"/>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292" s="2">
+        <v>45063</v>
+      </c>
+      <c r="B292" s="3"/>
+      <c r="C292" s="3"/>
+      <c r="D292" s="3"/>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293" s="2">
+        <v>45064</v>
+      </c>
+      <c r="B293" s="3"/>
+      <c r="C293" s="3"/>
+      <c r="D293" s="3"/>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A294" s="2">
+        <v>45065</v>
+      </c>
+      <c r="B294" s="3"/>
+      <c r="C294" s="3"/>
+      <c r="D294" s="3"/>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A295" s="2">
+        <v>45066</v>
+      </c>
+      <c r="B295" s="3"/>
+      <c r="C295" s="3"/>
+      <c r="D295" s="3"/>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296" s="2">
+        <v>45067</v>
+      </c>
+      <c r="B296" s="3"/>
+      <c r="C296" s="3"/>
+      <c r="D296" s="3"/>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298" s="2">
+        <v>45068</v>
+      </c>
+      <c r="B298" s="3"/>
+      <c r="C298" s="3"/>
+      <c r="D298" s="3"/>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299" s="2">
+        <v>45069</v>
+      </c>
+      <c r="B299" s="3"/>
+      <c r="C299" s="3"/>
+      <c r="D299" s="3"/>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A300" s="2">
+        <v>45070</v>
+      </c>
+      <c r="B300" s="3"/>
+      <c r="C300" s="3"/>
+      <c r="D300" s="3"/>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A301" s="2">
+        <v>45071</v>
+      </c>
+      <c r="B301" s="3"/>
+      <c r="C301" s="3"/>
+      <c r="D301" s="3"/>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A302" s="2">
+        <v>45072</v>
+      </c>
+      <c r="B302" s="3"/>
+      <c r="C302" s="3"/>
+      <c r="D302" s="3"/>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A303" s="2">
+        <v>45073</v>
+      </c>
+      <c r="B303" s="3"/>
+      <c r="C303" s="3"/>
+      <c r="D303" s="3"/>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A304" s="2">
+        <v>45074</v>
+      </c>
+      <c r="B304" s="3"/>
+      <c r="C304" s="3"/>
+      <c r="D304" s="3"/>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A306" s="2">
+        <v>45075</v>
+      </c>
+      <c r="B306" s="3"/>
+      <c r="C306" s="3"/>
+      <c r="D306" s="3"/>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A307" s="2">
+        <v>45076</v>
+      </c>
+      <c r="B307" s="3"/>
+      <c r="C307" s="3"/>
+      <c r="D307" s="3"/>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A308" s="2">
+        <v>45077</v>
+      </c>
+      <c r="B308" s="3"/>
+      <c r="C308" s="3"/>
+      <c r="D308" s="3"/>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A309" s="2">
+        <v>45078</v>
+      </c>
+      <c r="B309" s="3"/>
+      <c r="C309" s="3"/>
+      <c r="D309" s="3"/>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A310" s="2">
+        <v>45079</v>
+      </c>
+      <c r="B310" s="3"/>
+      <c r="C310" s="3"/>
+      <c r="D310" s="3"/>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A311" s="2">
+        <v>45080</v>
+      </c>
+      <c r="B311" s="3"/>
+      <c r="C311" s="3"/>
+      <c r="D311" s="3"/>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A312" s="2">
+        <v>45081</v>
+      </c>
+      <c r="B312" s="3"/>
+      <c r="C312" s="3"/>
+      <c r="D312" s="3"/>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A314" s="2">
+        <v>45082</v>
+      </c>
+      <c r="B314" s="3"/>
+      <c r="C314" s="3"/>
+      <c r="D314" s="3"/>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A315" s="2">
+        <v>45083</v>
+      </c>
+      <c r="B315" s="3"/>
+      <c r="C315" s="3"/>
+      <c r="D315" s="3"/>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A316" s="2">
+        <v>45084</v>
+      </c>
+      <c r="B316" s="3"/>
+      <c r="C316" s="3"/>
+      <c r="D316" s="3"/>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A317" s="2">
+        <v>45085</v>
+      </c>
+      <c r="B317" s="3"/>
+      <c r="C317" s="3"/>
+      <c r="D317" s="3"/>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A318" s="2">
+        <v>45086</v>
+      </c>
+      <c r="B318" s="3"/>
+      <c r="C318" s="3"/>
+      <c r="D318" s="3"/>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A319" s="2">
+        <v>45087</v>
+      </c>
+      <c r="B319" s="3"/>
+      <c r="C319" s="3"/>
+      <c r="D319" s="3"/>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A320" s="2">
+        <v>45088</v>
+      </c>
+      <c r="B320" s="3"/>
+      <c r="C320" s="3"/>
+      <c r="D320" s="3"/>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A322" s="2">
+        <v>45089</v>
+      </c>
+      <c r="B322" s="3"/>
+      <c r="C322" s="3"/>
+      <c r="D322" s="3"/>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A323" s="2">
+        <v>45090</v>
+      </c>
+      <c r="B323" s="3"/>
+      <c r="C323" s="3"/>
+      <c r="D323" s="3"/>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A324" s="2">
+        <v>45091</v>
+      </c>
+      <c r="B324" s="3"/>
+      <c r="C324" s="3"/>
+      <c r="D324" s="3"/>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A325" s="2">
+        <v>45092</v>
+      </c>
+      <c r="B325" s="3"/>
+      <c r="C325" s="3"/>
+      <c r="D325" s="3"/>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A326" s="2">
+        <v>45093</v>
+      </c>
+      <c r="B326" s="3"/>
+      <c r="C326" s="3"/>
+      <c r="D326" s="3"/>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A327" s="2">
+        <v>45094</v>
+      </c>
+      <c r="B327" s="3"/>
+      <c r="C327" s="3"/>
+      <c r="D327" s="3"/>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A328" s="2">
+        <v>45095</v>
+      </c>
+      <c r="B328" s="3"/>
+      <c r="C328" s="3"/>
+      <c r="D328" s="3"/>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A330" s="2">
+        <v>45096</v>
+      </c>
+      <c r="B330" s="3"/>
+      <c r="C330" s="3"/>
+      <c r="D330" s="3"/>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A331" s="2">
+        <v>45097</v>
+      </c>
+      <c r="B331" s="3"/>
+      <c r="C331" s="3"/>
+      <c r="D331" s="3"/>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A332" s="2">
+        <v>45098</v>
+      </c>
+      <c r="B332" s="3"/>
+      <c r="C332" s="3"/>
+      <c r="D332" s="3"/>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A333" s="2">
+        <v>45099</v>
+      </c>
+      <c r="B333" s="3"/>
+      <c r="C333" s="3"/>
+      <c r="D333" s="3"/>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A334" s="2">
+        <v>45100</v>
+      </c>
+      <c r="B334" s="3"/>
+      <c r="C334" s="3"/>
+      <c r="D334" s="3"/>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A335" s="2">
+        <v>45101</v>
+      </c>
+      <c r="B335" s="3"/>
+      <c r="C335" s="3"/>
+      <c r="D335" s="3"/>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A336" s="2">
+        <v>45102</v>
+      </c>
+      <c r="B336" s="3"/>
+      <c r="C336" s="3"/>
+      <c r="D336" s="3"/>
+    </row>
+    <row r="338" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B338" s="3">
+        <f>SUM(B2:B287)</f>
+        <v>1219</v>
+      </c>
+      <c r="C338">
+        <f>B338/31</f>
+        <v>39.322580645161288</v>
+      </c>
+      <c r="D338">
+        <f>35*7</f>
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>